<commit_message>
Final report finished, comment about performance added to the primary table SQL query.
</commit_message>
<xml_diff>
--- a/SQL project/Engeto_SQL projekt_finální zpráva.xlsx
+++ b/SQL project/Engeto_SQL projekt_finální zpráva.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VV\Desktop\Engeto\SQL project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F1E455-1401-4A2F-B572-41E491334314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE88E323-F4DC-4A8F-88D1-8306F8DCC49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="7" activeTab="9" xr2:uid="{9FAA7287-DE81-4884-B732-C7116C800970}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{9FAA7287-DE81-4884-B732-C7116C800970}"/>
   </bookViews>
   <sheets>
     <sheet name="data_Engeto_SQL project_Query 1" sheetId="2" r:id="rId1"/>
@@ -38,8 +38,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId11"/>
-    <pivotCache cacheId="14" r:id="rId12"/>
+    <pivotCache cacheId="0" r:id="rId11"/>
+    <pivotCache cacheId="1" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="769">
   <si>
     <t xml:space="preserve">rok  </t>
   </si>
@@ -2333,9 +2333,6 @@
     <t>4. Existuje rok, ve kterém byl meziroční nárůst cen potravin výrazně vyšší než růst mezd (větší než 10 %)?</t>
   </si>
   <si>
-    <t>Ve sledovaném období let 2006 až 2018 nebyl v žádném roce meziroční nárůst cen potravin o 10% vyšší než růst průměrných mezd. Nejvýše vzrostla průěrná cena potravin v roce 2017 a to o 9,628 %.</t>
-  </si>
-  <si>
     <t xml:space="preserve">region        </t>
   </si>
   <si>
@@ -2408,9 +2405,6 @@
     <t xml:space="preserve">3.20 %                       </t>
   </si>
   <si>
-    <t>5. Má výška HDP vliv na změny ve mzdách a cenách potravin? Neboli, pokud HDP vzroste výrazněji v jednom roce, projeví se to na cenách potravin či mzdách ve stejném nebo násdujícím roce výraznějším růstem?</t>
-  </si>
-  <si>
     <t>Změny cen (%)</t>
   </si>
   <si>
@@ -2466,6 +2460,18 @@
   </si>
   <si>
     <t>Změna cen (%)</t>
+  </si>
+  <si>
+    <t>Poměr růstu cen a platů</t>
+  </si>
+  <si>
+    <t>Průměrná hodnota poměru</t>
+  </si>
+  <si>
+    <t>5. Má výška HDP vliv na změny ve mzdách a cenách potravin? Neboli, pokud HDP vzroste výrazněji v jednom roce, projeví se to na cenách potravin či mzdách ve stejném nebo následujícím roce výraznějším růstem?</t>
+  </si>
+  <si>
+    <t>Pro účely studie jsem za významné meziroční procentní změny považoval změny vyšší než 2,5% pro HDP a 5 % pro platy a ceny potravin. Ve sledovaném období let 2006 až 2018 došlo k takovým významným změnám v letech 2007, 2008, 2009, 2015, 2016, 2017 a 2018. S vyjímkou roku 2009 došlo ve všech těchto letech jak k růstu HDP, tak i k růstu platů a cen potravin, přičemž růst cen potravin byl vždy přibližně dvojnásobný oproti růstu platů (průměrná hodnota poměru růstu cen potravin vůči růstu platů je 2,12). V roce 2009 došlo vlivem celosvětové finanční krize ke kontrakci HDP o 4,66 %, ale tato kontrakce se neodrazila v poklesu platů a cen potravin, jak by se dalo čekat. Tento jev byl zřejmě zapříčiněn v tu dobu nízkou nezaměstnaností ve výši 7,12 % (dle dat ČSÚ), která dále tlačila na růst mezd. To, že v roce 2009 rostly ceny potravin i přes pokles HDP by bylo možné vysvětlit tím, že platy také vzrostly.</t>
   </si>
 </sst>
 </file>
@@ -2741,7 +2747,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2862,6 +2868,24 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2954,13 +2978,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="146">
+  <dxfs count="155">
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -2973,12 +3065,23 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3006,7 +3109,7 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -3016,15 +3119,7 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3052,7 +3147,7 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -3062,15 +3157,7 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3094,6 +3181,95 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3890,209 +4066,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
     <dxf>
@@ -4303,6 +4276,209 @@
     </dxf>
     <dxf>
       <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
     <dxf>
       <alignment vertical="center"/>
@@ -4370,7 +4546,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Engeto_SQL projekt_finální zpráva.xlsx]Qry2_Odpověď!PivotTable16</c:name>
+    <c:name>[Engeto_SQL projekt_Finální zpráva.xlsx]Qry2_Odpověď!PivotTable16</c:name>
     <c:fmtId val="1"/>
   </c:pivotSource>
   <c:chart>
@@ -6551,14 +6727,61 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.68159127715418555"/>
-          <c:y val="1.9111859115500902E-2"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="cs-CZ" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Změny</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="cs-CZ" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="cs-CZ" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>HDP, platů</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="cs-CZ" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> a cen v letech 2007, 2008, 2009, 2015, 2016, 2017, 2018 </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6574,10 +6797,7 @@
           <a:pPr>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -6601,8 +6821,9 @@
           <c:h val="0.7894149645480657"/>
         </c:manualLayout>
       </c:layout>
-      <c:radarChart>
-        <c:radarStyle val="marker"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -6619,24 +6840,24 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="3175">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.5957446808510575E-2"/>
-                  <c:y val="3.3445753452126581E-2"/>
+                  <c:x val="-1.1233458063062288E-2"/>
+                  <c:y val="-9.5559295577505397E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -6648,16 +6869,16 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-FC4B-4A9A-8C11-78A5675863D5}"/>
+                  <c16:uniqueId val="{00000000-E809-4EA6-9544-E57E8EFAD475}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="2"/>
+              <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.1276595744680916E-2"/>
-                  <c:y val="-4.7779647788752256E-3"/>
+                  <c:x val="-9.8713551186215484E-3"/>
+                  <c:y val="-1.1944911947188065E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -6669,16 +6890,16 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-FC4B-4A9A-8C11-78A5675863D5}"/>
+                  <c16:uniqueId val="{00000001-E809-4EA6-9544-E57E8EFAD475}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="3"/>
+              <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="7.9787234042553196E-2"/>
-                  <c:y val="9.0781330798629295E-2"/>
+                  <c:x val="-1.4184397163120697E-2"/>
+                  <c:y val="-1.1944911947188065E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -6690,14 +6911,102 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000000-FC4B-4A9A-8C11-78A5675863D5}"/>
+                  <c16:uniqueId val="{00000002-E809-4EA6-9544-E57E8EFAD475}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.4791943358239214E-2"/>
+                  <c:y val="1.433389433662559E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-E809-4EA6-9544-E57E8EFAD475}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1258188982444593E-2"/>
+                  <c:y val="-1.4333894336625765E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-E809-4EA6-9544-E57E8EFAD475}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0779827283063792E-2"/>
+                  <c:y val="-2.3889823894376128E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-E809-4EA6-9544-E57E8EFAD475}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1865652998740712E-2"/>
+                  <c:y val="-9.5559295577504512E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-E809-4EA6-9544-E57E8EFAD475}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="6350">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -6710,10 +7019,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="bg1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -6812,7 +7118,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-62D8-43BE-ACD2-6D0023584897}"/>
+              <c16:uniqueId val="{00000007-E809-4EA6-9544-E57E8EFAD475}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6831,22 +7137,173 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln w="3175">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.2859386304829681E-2"/>
+                  <c:y val="-2.388982389437613E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-E809-4EA6-9544-E57E8EFAD475}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.7792627090335961E-3"/>
+                  <c:y val="-4.7779647788752256E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-E809-4EA6-9544-E57E8EFAD475}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.4583027619681005E-2"/>
+                  <c:y val="-4.7779647788752256E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-E809-4EA6-9544-E57E8EFAD475}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1883552650181831E-2"/>
+                  <c:y val="-2.8667788673251354E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-E809-4EA6-9544-E57E8EFAD475}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.614159437124283E-2"/>
+                  <c:y val="-9.5559295577504512E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-E809-4EA6-9544-E57E8EFAD475}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.5810407583710648E-2"/>
+                  <c:y val="-1.672287672606329E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-E809-4EA6-9544-E57E8EFAD475}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0834823313578367E-2"/>
+                  <c:y val="-1.1944911947188152E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-E809-4EA6-9544-E57E8EFAD475}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
+              <a:ln w="6350">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -6961,7 +7418,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-62D8-43BE-ACD2-6D0023584897}"/>
+              <c16:uniqueId val="{0000000F-E809-4EA6-9544-E57E8EFAD475}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6980,24 +7437,24 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln w="3175">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="3.0141843971631142E-2"/>
-                  <c:y val="6.4502524514815543E-2"/>
+                  <c:x val="-1.2947414542351713E-3"/>
+                  <c:y val="-4.7779647788752473E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -7009,16 +7466,16 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-FC4B-4A9A-8C11-78A5675863D5}"/>
+                  <c16:uniqueId val="{00000010-E809-4EA6-9544-E57E8EFAD475}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="2"/>
+              <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.5957446808510637E-2"/>
-                  <c:y val="-4.7779647788752256E-3"/>
+                  <c:x val="-7.0922396709715068E-3"/>
+                  <c:y val="-9.5559295577504512E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -7030,16 +7487,16 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-FC4B-4A9A-8C11-78A5675863D5}"/>
+                  <c16:uniqueId val="{00000011-E809-4EA6-9544-E57E8EFAD475}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="4"/>
+              <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.5957446808510637E-2"/>
-                  <c:y val="-5.0168630178189871E-2"/>
+                  <c:x val="-5.1473171578708616E-3"/>
+                  <c:y val="-1.6722876726063332E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -7051,16 +7508,16 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-FC4B-4A9A-8C11-78A5675863D5}"/>
+                  <c16:uniqueId val="{00000012-E809-4EA6-9544-E57E8EFAD475}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="5"/>
+              <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="3.3687943262411348E-2"/>
-                  <c:y val="-8.7595009041026585E-17"/>
+                  <c:x val="-1.9055432799304006E-2"/>
+                  <c:y val="-1.672287672606327E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -7072,16 +7529,16 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-FC4B-4A9A-8C11-78A5675863D5}"/>
+                  <c16:uniqueId val="{00000013-E809-4EA6-9544-E57E8EFAD475}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="6"/>
+              <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="2.3049645390070889E-2"/>
-                  <c:y val="2.388982389437613E-2"/>
+                  <c:x val="-8.4542561436662337E-3"/>
+                  <c:y val="-1.1944911947187976E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -7093,15 +7550,59 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-FC4B-4A9A-8C11-78A5675863D5}"/>
+                  <c16:uniqueId val="{00000014-E809-4EA6-9544-E57E8EFAD475}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1761195129461607E-2"/>
+                  <c:y val="-1.433389433662572E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000015-E809-4EA6-9544-E57E8EFAD475}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.8712078572379141E-3"/>
+                  <c:y val="-4.7779647788752698E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000016-E809-4EA6-9544-E57E8EFAD475}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
-              <a:noFill/>
-              <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="6350">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -7217,7 +7718,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-62D8-43BE-ACD2-6D0023584897}"/>
+              <c16:uniqueId val="{00000017-E809-4EA6-9544-E57E8EFAD475}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7229,9 +7730,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="28554080"/>
         <c:axId val="28555520"/>
-      </c:radarChart>
+      </c:barChart>
       <c:catAx>
         <c:axId val="28554080"/>
         <c:scaling>
@@ -7277,10 +7779,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -7382,12 +7881,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -7409,8 +7905,7 @@
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
         <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
+          <a:alpha val="99000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:round/>
@@ -9181,24 +9676,26 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>17929</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>457201</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>8965</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>8964</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>188260</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EBF8A01-78CA-8B74-AAC8-E86533870A00}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A32D11F-51D4-4C46-8525-83ED8B77D36D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -9210,6 +9707,50 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>28765</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>17929</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>147845</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E75C2FF2-4C57-849B-10E7-D071F3525325}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="8114930"/>
+          <a:ext cx="11582400" cy="5246891"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -12082,7 +12623,629 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F400FEAB-C540-466A-B80E-A4C59DAC6285}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Celkem" missingCaption="0" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" mergeItem="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Odvětví" colHeaderCaption="Roky">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1A8902DF-7E1F-42F6-BF1E-36EF257AF7BC}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Celkem" missingCaption="0" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" mergeItem="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Odvětví" colHeaderCaption="Roky">
+  <location ref="A3:N23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField axis="axisCol" showAll="0">
+      <items count="27">
+        <item m="1" x="13"/>
+        <item m="1" x="14"/>
+        <item m="1" x="15"/>
+        <item m="1" x="16"/>
+        <item m="1" x="17"/>
+        <item m="1" x="18"/>
+        <item m="1" x="19"/>
+        <item m="1" x="20"/>
+        <item m="1" x="21"/>
+        <item m="1" x="22"/>
+        <item m="1" x="23"/>
+        <item m="1" x="24"/>
+        <item m="1" x="25"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="20">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="19">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="13">
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Průměrný plat v Kč" fld="2" subtotal="average" baseField="1" baseItem="0" numFmtId="4"/>
+  </dataFields>
+  <formats count="17">
+    <format dxfId="113">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="12" selected="0">
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+            <x v="10"/>
+            <x v="11"/>
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="112">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="111">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="12">
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+            <x v="10"/>
+            <x v="11"/>
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="110">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="109">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="108">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="107">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="106">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="105">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="104">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="103">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="102">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="101">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="100">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="99">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="98">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="97">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <conditionalFormats count="1">
+    <conditionalFormat priority="2">
+      <pivotAreas count="1">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
+  <pivotTableStyleInfo name="PivotStyleLight21" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DFD2BA96-6C5F-4529-9B0E-F24753144630}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Celkem" missingCaption="0" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" mergeItem="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Odvětví" colHeaderCaption="Roky">
+  <location ref="A47:N67" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField axis="axisCol" showAll="0">
+      <items count="27">
+        <item m="1" x="13"/>
+        <item m="1" x="14"/>
+        <item m="1" x="15"/>
+        <item m="1" x="16"/>
+        <item m="1" x="17"/>
+        <item m="1" x="18"/>
+        <item m="1" x="19"/>
+        <item m="1" x="20"/>
+        <item m="1" x="21"/>
+        <item m="1" x="22"/>
+        <item m="1" x="23"/>
+        <item m="1" x="24"/>
+        <item m="1" x="25"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="20">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="19">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="13">
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Průměrná změna platu v %" fld="8" subtotal="average" baseField="1" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <formats count="17">
+    <format dxfId="130">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="12" selected="0">
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+            <x v="10"/>
+            <x v="11"/>
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="129">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="128">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="12">
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+            <x v="10"/>
+            <x v="11"/>
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="127">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="126">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="125">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="124">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="123">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="122">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="121">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="120">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="119">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="118">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="117">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="116">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="115">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="114">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <conditionalFormats count="1">
+    <conditionalFormat priority="4">
+      <pivotAreas count="1">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
+  <pivotTableStyleInfo name="PivotStyleLight21" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F400FEAB-C540-466A-B80E-A4C59DAC6285}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Celkem" missingCaption="0" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" mergeItem="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Odvětví" colHeaderCaption="Roky">
   <location ref="A25:N45" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisCol" showAll="0">
@@ -12258,7 +13421,7 @@
     <dataField name="Průměrná změna platu v Kč" fld="7" subtotal="average" baseField="1" baseItem="0" numFmtId="4"/>
   </dataFields>
   <formats count="17">
-    <format dxfId="104">
+    <format dxfId="147">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="12" selected="0">
@@ -12278,10 +13441,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="103">
+    <format dxfId="146">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="102">
+    <format dxfId="145">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="12">
@@ -12301,7 +13464,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="101">
+    <format dxfId="144">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -12313,13 +13476,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="100">
+    <format dxfId="143">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="99">
+    <format dxfId="142">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="98">
+    <format dxfId="141">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -12328,38 +13491,38 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="97">
+    <format dxfId="140">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="96">
+    <format dxfId="139">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="95">
+    <format dxfId="138">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="94">
+    <format dxfId="137">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="93">
+    <format dxfId="136">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="92">
+    <format dxfId="135">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="91">
+    <format dxfId="134">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="90">
+    <format dxfId="133">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="89">
+    <format dxfId="132">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="131">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
@@ -12588,630 +13751,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1A8902DF-7E1F-42F6-BF1E-36EF257AF7BC}" name="PivotTable6" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Celkem" missingCaption="0" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" mergeItem="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Odvětví" colHeaderCaption="Roky">
-  <location ref="A3:N23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField axis="axisCol" showAll="0">
-      <items count="27">
-        <item m="1" x="13"/>
-        <item m="1" x="14"/>
-        <item m="1" x="15"/>
-        <item m="1" x="16"/>
-        <item m="1" x="17"/>
-        <item m="1" x="18"/>
-        <item m="1" x="19"/>
-        <item m="1" x="20"/>
-        <item m="1" x="21"/>
-        <item m="1" x="22"/>
-        <item m="1" x="23"/>
-        <item m="1" x="24"/>
-        <item m="1" x="25"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="20">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="19">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="13">
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Průměrný plat v Kč" fld="2" subtotal="average" baseField="1" baseItem="0" numFmtId="4"/>
-  </dataFields>
-  <formats count="17">
-    <format dxfId="121">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="12" selected="0">
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="5"/>
-            <x v="6"/>
-            <x v="7"/>
-            <x v="8"/>
-            <x v="9"/>
-            <x v="10"/>
-            <x v="11"/>
-            <x v="12"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="120">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="119">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="12">
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="5"/>
-            <x v="6"/>
-            <x v="7"/>
-            <x v="8"/>
-            <x v="9"/>
-            <x v="10"/>
-            <x v="11"/>
-            <x v="12"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="118">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="117">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="116">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="115">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="114">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="113">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="112">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="111">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="110">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="109">
-      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
-    </format>
-    <format dxfId="108">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="107">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="106">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="105">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <conditionalFormats count="1">
-    <conditionalFormat priority="2">
-      <pivotAreas count="1">
-        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-  </conditionalFormats>
-  <pivotTableStyleInfo name="PivotStyleLight21" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DFD2BA96-6C5F-4529-9B0E-F24753144630}" name="PivotTable5" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Celkem" missingCaption="0" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" mergeItem="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Odvětví" colHeaderCaption="Roky">
-  <location ref="A47:N67" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField axis="axisCol" showAll="0">
-      <items count="27">
-        <item m="1" x="13"/>
-        <item m="1" x="14"/>
-        <item m="1" x="15"/>
-        <item m="1" x="16"/>
-        <item m="1" x="17"/>
-        <item m="1" x="18"/>
-        <item m="1" x="19"/>
-        <item m="1" x="20"/>
-        <item m="1" x="21"/>
-        <item m="1" x="22"/>
-        <item m="1" x="23"/>
-        <item m="1" x="24"/>
-        <item m="1" x="25"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="20">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="19">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="13">
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Průměrná změna platu v %" fld="8" subtotal="average" baseField="1" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <formats count="17">
-    <format dxfId="138">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="12" selected="0">
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="5"/>
-            <x v="6"/>
-            <x v="7"/>
-            <x v="8"/>
-            <x v="9"/>
-            <x v="10"/>
-            <x v="11"/>
-            <x v="12"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="137">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="136">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="12">
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="5"/>
-            <x v="6"/>
-            <x v="7"/>
-            <x v="8"/>
-            <x v="9"/>
-            <x v="10"/>
-            <x v="11"/>
-            <x v="12"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="135">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="134">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="133">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="132">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="131">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="130">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="129">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="128">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="127">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="126">
-      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
-    </format>
-    <format dxfId="125">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="124">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="123">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="122">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <conditionalFormats count="1">
-    <conditionalFormat priority="4">
-      <pivotAreas count="1">
-        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-  </conditionalFormats>
-  <pivotTableStyleInfo name="PivotStyleLight21" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4094ADC6-FE8E-4B5F-9B5D-D856087DA508}" name="PivotTable16" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10" rowHeaderCaption="Rok" colHeaderCaption="Název potraviny">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4094ADC6-FE8E-4B5F-9B5D-D856087DA508}" name="PivotTable16" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10" rowHeaderCaption="Rok" colHeaderCaption="Název potraviny">
   <location ref="A3:C6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -13256,37 +13797,72 @@
     <dataField name="Množství potraviny za průměrný plat" fld="2" baseField="0" baseItem="0" numFmtId="4"/>
   </dataFields>
   <formats count="29">
-    <format dxfId="75">
+    <format dxfId="84">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="74">
+    <format dxfId="83">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="73">
+    <format dxfId="82">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="72">
+    <format dxfId="81">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="71">
+    <format dxfId="80">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="70">
+    <format dxfId="79">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="69">
+    <format dxfId="78">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="77">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
+    </format>
+    <format dxfId="76">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="75">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="74">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="73">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="72">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="71">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="70">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="69">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="68">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
     <format dxfId="67">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
@@ -13321,54 +13897,19 @@
       </pivotArea>
     </format>
     <format dxfId="59">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
     <format dxfId="58">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="57">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="56">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="55">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
-    </format>
-    <format dxfId="54">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="53">
-      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="52">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="51">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="50">
-      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="49">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="48">
+    <format dxfId="57">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="56">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
   </formats>
@@ -13533,13 +14074,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{59717E4D-993C-474C-8317-F90BA6AA268D}" name="data_Engeto_SQL_project_Query_1" displayName="data_Engeto_SQL_project_Query_1" ref="A1:I248" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:I248" xr:uid="{59717E4D-993C-474C-8317-F90BA6AA268D}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{CDAA9260-8D45-427D-A6B3-E5207BFE4E4F}" uniqueName="1" name="rok  " queryTableFieldId="1" dataDxfId="145"/>
-    <tableColumn id="2" xr3:uid="{5AAC1FB1-8893-4D43-8F2E-B2749375C45C}" uniqueName="2" name="odvetvi                                                     " queryTableFieldId="2" dataDxfId="144"/>
-    <tableColumn id="4" xr3:uid="{6FF168BE-4CDD-464B-A04B-91087C4C72AC}" uniqueName="4" name="prumerny_plat " queryTableFieldId="4" dataDxfId="143"/>
-    <tableColumn id="5" xr3:uid="{FEF4ABEF-BC71-4B22-B93B-16F57CBEDBE0}" uniqueName="5" name="mezirocni_trend" queryTableFieldId="5" dataDxfId="142"/>
-    <tableColumn id="6" xr3:uid="{3339668B-12D2-430C-BC6B-1C66C07F6118}" uniqueName="6" name="prumerny_plat_predchozi_rok" queryTableFieldId="6" dataDxfId="141"/>
-    <tableColumn id="7" xr3:uid="{426B1E04-62A3-4FF1-ABA9-DAF85555A826}" uniqueName="7" name="prumerna_mezirocni_zmena_platu_abs" queryTableFieldId="7" dataDxfId="140"/>
-    <tableColumn id="8" xr3:uid="{756220FA-1DFF-4FF8-B0E0-2A11782600CF}" uniqueName="8" name="prumerna_mezirocni_zmena_platu_procentne" queryTableFieldId="8" dataDxfId="139"/>
+    <tableColumn id="1" xr3:uid="{CDAA9260-8D45-427D-A6B3-E5207BFE4E4F}" uniqueName="1" name="rok  " queryTableFieldId="1" dataDxfId="154"/>
+    <tableColumn id="2" xr3:uid="{5AAC1FB1-8893-4D43-8F2E-B2749375C45C}" uniqueName="2" name="odvetvi                                                     " queryTableFieldId="2" dataDxfId="153"/>
+    <tableColumn id="4" xr3:uid="{6FF168BE-4CDD-464B-A04B-91087C4C72AC}" uniqueName="4" name="prumerny_plat " queryTableFieldId="4" dataDxfId="152"/>
+    <tableColumn id="5" xr3:uid="{FEF4ABEF-BC71-4B22-B93B-16F57CBEDBE0}" uniqueName="5" name="mezirocni_trend" queryTableFieldId="5" dataDxfId="151"/>
+    <tableColumn id="6" xr3:uid="{3339668B-12D2-430C-BC6B-1C66C07F6118}" uniqueName="6" name="prumerny_plat_predchozi_rok" queryTableFieldId="6" dataDxfId="150"/>
+    <tableColumn id="7" xr3:uid="{426B1E04-62A3-4FF1-ABA9-DAF85555A826}" uniqueName="7" name="prumerna_mezirocni_zmena_platu_abs" queryTableFieldId="7" dataDxfId="149"/>
+    <tableColumn id="8" xr3:uid="{756220FA-1DFF-4FF8-B0E0-2A11782600CF}" uniqueName="8" name="prumerna_mezirocni_zmena_platu_procentne" queryTableFieldId="8" dataDxfId="148"/>
     <tableColumn id="10" xr3:uid="{1CB3FF3A-B16B-46F0-88AC-116FDEDD24E9}" uniqueName="10" name="Změna platu v Kč" queryTableFieldId="11"/>
     <tableColumn id="12" xr3:uid="{394FBDBE-0A92-4D7D-B2FE-4CF7F572D480}" uniqueName="12" name="Změna platu v %" queryTableFieldId="13"/>
   </tableColumns>
@@ -13548,26 +14089,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B1B24AEF-4280-47CF-B5FC-94027346278F}" name="data_Engeto_SQL_project_Query_2a_2" displayName="data_Engeto_SQL_project_Query_2a_2" ref="A1:E5" tableType="queryTable" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B1B24AEF-4280-47CF-B5FC-94027346278F}" name="data_Engeto_SQL_project_Query_2a_2" displayName="data_Engeto_SQL_project_Query_2a_2" ref="A1:E5" tableType="queryTable" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95">
   <autoFilter ref="A1:E5" xr:uid="{B1B24AEF-4280-47CF-B5FC-94027346278F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{032CCDCD-651A-4357-8ABF-3B314B15C573}" uniqueName="1" name="rok  " queryTableFieldId="1" dataDxfId="85"/>
-    <tableColumn id="2" xr3:uid="{EFF99841-F552-4F03-880A-313E48630FDF}" uniqueName="2" name="nazev_potraviny            " queryTableFieldId="2" dataDxfId="84"/>
-    <tableColumn id="3" xr3:uid="{A1E893A7-46DD-4F3B-8850-36019CC18E35}" uniqueName="3" name="prumerna_cena_potraviny" queryTableFieldId="3" dataDxfId="83"/>
-    <tableColumn id="4" xr3:uid="{6E6461B2-BA3B-4BF9-B81F-EE31F1EC4028}" uniqueName="4" name="prumerny_plat     " queryTableFieldId="4" dataDxfId="82"/>
-    <tableColumn id="5" xr3:uid="{2BC971FE-4E78-4AFC-BEF8-4107BD29E15F}" uniqueName="5" name="mnozstvi_potraviny_za_prumerny_plat" queryTableFieldId="5" dataDxfId="81"/>
+    <tableColumn id="1" xr3:uid="{032CCDCD-651A-4357-8ABF-3B314B15C573}" uniqueName="1" name="rok  " queryTableFieldId="1" dataDxfId="94"/>
+    <tableColumn id="2" xr3:uid="{EFF99841-F552-4F03-880A-313E48630FDF}" uniqueName="2" name="nazev_potraviny            " queryTableFieldId="2" dataDxfId="93"/>
+    <tableColumn id="3" xr3:uid="{A1E893A7-46DD-4F3B-8850-36019CC18E35}" uniqueName="3" name="prumerna_cena_potraviny" queryTableFieldId="3" dataDxfId="92"/>
+    <tableColumn id="4" xr3:uid="{6E6461B2-BA3B-4BF9-B81F-EE31F1EC4028}" uniqueName="4" name="prumerny_plat     " queryTableFieldId="4" dataDxfId="91"/>
+    <tableColumn id="5" xr3:uid="{2BC971FE-4E78-4AFC-BEF8-4107BD29E15F}" uniqueName="5" name="mnozstvi_potraviny_za_prumerny_plat" queryTableFieldId="5" dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0E11E358-3979-4857-ABC9-52BD7B36AB13}" name="data_Engeto_SQL_project_Query_2b" displayName="data_Engeto_SQL_project_Query_2b" ref="A7:C11" tableType="queryTable" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0E11E358-3979-4857-ABC9-52BD7B36AB13}" name="data_Engeto_SQL_project_Query_2b" displayName="data_Engeto_SQL_project_Query_2b" ref="A7:C11" tableType="queryTable" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
   <autoFilter ref="A7:C11" xr:uid="{0E11E358-3979-4857-ABC9-52BD7B36AB13}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{12057956-D1EB-458E-9D28-027670B6EF8D}" uniqueName="1" name="rok  " queryTableFieldId="1" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{4BAE2827-D467-4EB1-9692-2C6701C3A100}" uniqueName="2" name="nazev_potraviny            " queryTableFieldId="2" dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{5321FD9A-B618-461F-9853-D8F9EBE91D82}" uniqueName="5" name="mnozstvi_potraviny_za_prumerny_plat" queryTableFieldId="5" dataDxfId="76"/>
+    <tableColumn id="1" xr3:uid="{12057956-D1EB-458E-9D28-027670B6EF8D}" uniqueName="1" name="rok  " queryTableFieldId="1" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{4BAE2827-D467-4EB1-9692-2C6701C3A100}" uniqueName="2" name="nazev_potraviny            " queryTableFieldId="2" dataDxfId="86"/>
+    <tableColumn id="5" xr3:uid="{5321FD9A-B618-461F-9853-D8F9EBE91D82}" uniqueName="5" name="mnozstvi_potraviny_za_prumerny_plat" queryTableFieldId="5" dataDxfId="85"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13577,76 +14118,80 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{27C584E5-351A-43CA-9E20-1C2BED3754FC}" name="data_Engeto_SQL_project_Query_3b" displayName="data_Engeto_SQL_project_Query_3b" ref="A1:C28" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:C28" xr:uid="{27C584E5-351A-43CA-9E20-1C2BED3754FC}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E9FDCD0B-34BA-49BF-BFD5-D90A4C062FED}" uniqueName="1" name="nazev_potraviny                 " queryTableFieldId="1" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{570AAA8F-8E9A-4A56-901E-22F447810B57}" uniqueName="2" name="prumerna_mezirocni_zmena_ceny_potraviny_procentne" queryTableFieldId="2" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{BBE176F1-9512-45B9-A30B-C6BE9EF19982}" uniqueName="3" name="poradi" queryTableFieldId="3" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{E9FDCD0B-34BA-49BF-BFD5-D90A4C062FED}" uniqueName="1" name="nazev_potraviny                 " queryTableFieldId="1" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{570AAA8F-8E9A-4A56-901E-22F447810B57}" uniqueName="2" name="prumerna_mezirocni_zmena_ceny_potraviny_procentne" queryTableFieldId="2" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{BBE176F1-9512-45B9-A30B-C6BE9EF19982}" uniqueName="3" name="poradi" queryTableFieldId="3" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2389A781-F3DF-4CC1-A599-56C06F303360}" name="Table4" displayName="Table4" ref="A3:C6" totalsRowShown="0" headerRowDxfId="43" headerRowBorderDxfId="42" tableBorderDxfId="41" totalsRowBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2389A781-F3DF-4CC1-A599-56C06F303360}" name="Table4" displayName="Table4" ref="A3:C6" totalsRowShown="0" headerRowDxfId="52" headerRowBorderDxfId="51" tableBorderDxfId="50" totalsRowBorderDxfId="49">
   <autoFilter ref="A3:C6" xr:uid="{2389A781-F3DF-4CC1-A599-56C06F303360}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4FC87035-37E3-42E6-946B-FC43A6C9C95C}" name="nazev_potraviny                 " dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{E2A150A1-D961-49EC-AF48-30479DD65B9A}" name="prumerna_mezirocni_zmena_ceny_potraviny_procentne" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{FF5D9388-4D42-41A8-B4B4-8F92B21DE1BA}" name="poradi" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{4FC87035-37E3-42E6-946B-FC43A6C9C95C}" name="nazev_potraviny                 " dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{E2A150A1-D961-49EC-AF48-30479DD65B9A}" name="prumerna_mezirocni_zmena_ceny_potraviny_procentne" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{FF5D9388-4D42-41A8-B4B4-8F92B21DE1BA}" name="poradi" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{48F146E2-4129-413F-9B6F-4417B22013A7}" name="data_Engeto_SQL_project_Query_4" displayName="data_Engeto_SQL_project_Query_4" ref="A1:K14" tableType="queryTable" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{48F146E2-4129-413F-9B6F-4417B22013A7}" name="data_Engeto_SQL_project_Query_4" displayName="data_Engeto_SQL_project_Query_4" ref="A1:K14" tableType="queryTable" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
   <autoFilter ref="A1:K14" xr:uid="{48F146E2-4129-413F-9B6F-4417B22013A7}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{67C6AAE0-A64E-436F-9CCC-7BD703793433}" uniqueName="1" name="rok  " queryTableFieldId="1" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{77D7C2CA-2038-42CD-AA6D-E31DD15361CF}" uniqueName="2" name="prumerna_cena" queryTableFieldId="2" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{7D6816C7-7CE3-40E0-9CE3-DAF1AD091192}" uniqueName="3" name="prumerna_cena_predchozi_rok" queryTableFieldId="3" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{20AC24DB-4A99-47FF-934D-E4561711675F}" uniqueName="4" name="rozdil_prumernych_cen_abs" queryTableFieldId="4" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{6078983B-5EFB-4603-83FD-22A14484DF9D}" uniqueName="5" name="rozdil_prumernych_cen_procentne" queryTableFieldId="5" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{F1B76DCA-96EA-4E08-B983-607918C314BF}" uniqueName="6" name="trend_cen                      " queryTableFieldId="6" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{3F78F8B6-27E8-47E1-A63B-88E43E85A547}" uniqueName="7" name="prumerny_plat " queryTableFieldId="7" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{D949FA26-9C9E-4CCF-A6B4-04F105F3E92B}" uniqueName="8" name="prumerny_plat_predchozi_rok" queryTableFieldId="8" dataDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{AC2F56F1-B04E-490F-BB78-7AA876F92041}" uniqueName="9" name="rozdil_prumernych_platu_abs" queryTableFieldId="9" dataDxfId="26"/>
-    <tableColumn id="10" xr3:uid="{01D69ACD-EFD5-4492-8CB4-E7B8CB20CD9B}" uniqueName="10" name="rozdil_prumernych_platu_procentne" queryTableFieldId="10" dataDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{C0B6D170-1F58-46BE-B13D-FC601491626B}" uniqueName="11" name="trend_platu             " queryTableFieldId="11" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{67C6AAE0-A64E-436F-9CCC-7BD703793433}" uniqueName="1" name="rok  " queryTableFieldId="1" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{77D7C2CA-2038-42CD-AA6D-E31DD15361CF}" uniqueName="2" name="prumerna_cena" queryTableFieldId="2" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{7D6816C7-7CE3-40E0-9CE3-DAF1AD091192}" uniqueName="3" name="prumerna_cena_predchozi_rok" queryTableFieldId="3" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{20AC24DB-4A99-47FF-934D-E4561711675F}" uniqueName="4" name="rozdil_prumernych_cen_abs" queryTableFieldId="4" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{6078983B-5EFB-4603-83FD-22A14484DF9D}" uniqueName="5" name="rozdil_prumernych_cen_procentne" queryTableFieldId="5" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{F1B76DCA-96EA-4E08-B983-607918C314BF}" uniqueName="6" name="trend_cen                      " queryTableFieldId="6" dataDxfId="38"/>
+    <tableColumn id="7" xr3:uid="{3F78F8B6-27E8-47E1-A63B-88E43E85A547}" uniqueName="7" name="prumerny_plat " queryTableFieldId="7" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{D949FA26-9C9E-4CCF-A6B4-04F105F3E92B}" uniqueName="8" name="prumerny_plat_predchozi_rok" queryTableFieldId="8" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{AC2F56F1-B04E-490F-BB78-7AA876F92041}" uniqueName="9" name="rozdil_prumernych_platu_abs" queryTableFieldId="9" dataDxfId="35"/>
+    <tableColumn id="10" xr3:uid="{01D69ACD-EFD5-4492-8CB4-E7B8CB20CD9B}" uniqueName="10" name="rozdil_prumernych_platu_procentne" queryTableFieldId="10" dataDxfId="34"/>
+    <tableColumn id="11" xr3:uid="{C0B6D170-1F58-46BE-B13D-FC601491626B}" uniqueName="11" name="trend_platu             " queryTableFieldId="11" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7E6A55AA-1E67-4718-8A28-74D241CAD387}" name="data_Engeto_SQL_project_Query_5" displayName="data_Engeto_SQL_project_Query_5" ref="A1:J8" tableType="queryTable" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7E6A55AA-1E67-4718-8A28-74D241CAD387}" name="data_Engeto_SQL_project_Query_5" displayName="data_Engeto_SQL_project_Query_5" ref="A1:J8" tableType="queryTable" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A1:J8" xr:uid="{7E6A55AA-1E67-4718-8A28-74D241CAD387}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{FE9A6C8C-993E-438B-9AEA-9D3224C81297}" uniqueName="1" name="region        " queryTableFieldId="1" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{781A05C4-7625-438F-AD1D-590F6171EE57}" uniqueName="2" name="stat          " queryTableFieldId="2" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{78E89A85-51B3-41CB-ABD4-3F08153F932B}" uniqueName="3" name="zkratka_meny" queryTableFieldId="3" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{755EE6A4-609D-4E47-B869-BFC624BDAAE4}" uniqueName="4" name="rok  " queryTableFieldId="4" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{3C2F9BAF-E6F9-48C9-97D8-2864750C914D}" uniqueName="8" name="mezirocni_zmena_HDP_procentni" queryTableFieldId="8" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{8B707BA1-2AAE-457F-A520-4221976655BF}" uniqueName="9" name="trend_HDP               " queryTableFieldId="9" dataDxfId="16"/>
-    <tableColumn id="14" xr3:uid="{3A1777C6-4A00-4095-946A-36EFDF68BD04}" uniqueName="14" name="mezirocni_zmena_platu_procentne" queryTableFieldId="14" dataDxfId="15"/>
-    <tableColumn id="15" xr3:uid="{5F1C61CC-14E5-49AC-B18E-8CE3171C7328}" uniqueName="15" name="trend_platu            " queryTableFieldId="15" dataDxfId="14"/>
-    <tableColumn id="20" xr3:uid="{C6A54F29-4212-4E39-9D68-01D5ECF517E1}" uniqueName="20" name="mezirocni_zmena_cen_procentne" queryTableFieldId="20" dataDxfId="13"/>
-    <tableColumn id="21" xr3:uid="{335706D2-03DD-4EBA-A511-31C3F9445D24}" uniqueName="21" name="trend_cen                     " queryTableFieldId="21" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{FE9A6C8C-993E-438B-9AEA-9D3224C81297}" uniqueName="1" name="region        " queryTableFieldId="1" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{781A05C4-7625-438F-AD1D-590F6171EE57}" uniqueName="2" name="stat          " queryTableFieldId="2" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{78E89A85-51B3-41CB-ABD4-3F08153F932B}" uniqueName="3" name="zkratka_meny" queryTableFieldId="3" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{755EE6A4-609D-4E47-B869-BFC624BDAAE4}" uniqueName="4" name="rok  " queryTableFieldId="4" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{3C2F9BAF-E6F9-48C9-97D8-2864750C914D}" uniqueName="8" name="mezirocni_zmena_HDP_procentni" queryTableFieldId="8" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{8B707BA1-2AAE-457F-A520-4221976655BF}" uniqueName="9" name="trend_HDP               " queryTableFieldId="9" dataDxfId="25"/>
+    <tableColumn id="14" xr3:uid="{3A1777C6-4A00-4095-946A-36EFDF68BD04}" uniqueName="14" name="mezirocni_zmena_platu_procentne" queryTableFieldId="14" dataDxfId="24"/>
+    <tableColumn id="15" xr3:uid="{5F1C61CC-14E5-49AC-B18E-8CE3171C7328}" uniqueName="15" name="trend_platu            " queryTableFieldId="15" dataDxfId="23"/>
+    <tableColumn id="20" xr3:uid="{C6A54F29-4212-4E39-9D68-01D5ECF517E1}" uniqueName="20" name="mezirocni_zmena_cen_procentne" queryTableFieldId="20" dataDxfId="22"/>
+    <tableColumn id="21" xr3:uid="{335706D2-03DD-4EBA-A511-31C3F9445D24}" uniqueName="21" name="trend_cen                     " queryTableFieldId="21" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{C696EF49-D3B7-4035-A657-9AE7E7E6138B}" name="Table15" displayName="Table15" ref="A5:G12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="A5:G12" xr:uid="{C696EF49-D3B7-4035-A657-9AE7E7E6138B}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{E4108C3D-3079-4479-B050-7FD29B380400}" name="region        " dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{F2030460-6D82-4DE8-822F-1771CD2C79A3}" name="stat          " dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{11FB66C7-6E9A-4F8E-924F-75C7783ADAA7}" name="zkratka_meny" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{53CCD221-6FD5-487B-B06D-C56164B8E381}" name="rok  " dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{AC7E035F-313D-4AA8-B0B7-DB62CC3A9E17}" name="Změna HDP (%)" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{44DB06D0-A627-4FF4-A2DC-DB4253FC21AE}" name="Změna platů (%)" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{2B3D24AD-13A2-4832-8780-1DDF1CCE5AEC}" name="Změna cen (%)" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{C696EF49-D3B7-4035-A657-9AE7E7E6138B}" name="Table15" displayName="Table15" ref="A5:H13" totalsRowCount="1" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+  <autoFilter ref="A5:H12" xr:uid="{C696EF49-D3B7-4035-A657-9AE7E7E6138B}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{E4108C3D-3079-4479-B050-7FD29B380400}" name="region        " dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{F2030460-6D82-4DE8-822F-1771CD2C79A3}" name="stat          " dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{11FB66C7-6E9A-4F8E-924F-75C7783ADAA7}" name="zkratka_meny" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{53CCD221-6FD5-487B-B06D-C56164B8E381}" name="rok  " dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{AC7E035F-313D-4AA8-B0B7-DB62CC3A9E17}" name="Změna HDP (%)" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{44DB06D0-A627-4FF4-A2DC-DB4253FC21AE}" name="Změna platů (%)" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{2B3D24AD-13A2-4832-8780-1DDF1CCE5AEC}" name="Změna cen (%)" totalsRowLabel="Průměrná hodnota poměru" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{9F552489-E927-4C43-BFA2-86B5BCB10CA1}" name="Poměr růstu cen a platů" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
+      <calculatedColumnFormula>Table15[[#This Row],[Změna cen (%)]]/Table15[[#This Row],[Změna platů (%)]]</calculatedColumnFormula>
+      <totalsRowFormula>AVERAGE(Table15[Poměr růstu cen a platů])</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13954,7 +14499,7 @@
   </sheetPr>
   <dimension ref="A1:I248"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -21007,10 +21552,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -21021,72 +21566,74 @@
     <col min="4" max="4" width="9.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.69921875" customWidth="1"/>
     <col min="6" max="7" width="31.8984375" customWidth="1"/>
-    <col min="8" max="8" width="21.296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.59765625" customWidth="1"/>
-    <col min="10" max="10" width="26.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.8984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
-        <v>747</v>
-      </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="79"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="81"/>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="83" t="s">
+        <v>767</v>
+      </c>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="85"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="87"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
+        <v>722</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>723</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="C5" s="16" t="s">
         <v>724</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>725</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="16" t="s">
+        <v>762</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>763</v>
+      </c>
+      <c r="G5" s="37" t="s">
         <v>764</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="H5" s="16" t="s">
         <v>765</v>
       </c>
-      <c r="G5" s="37" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
+        <v>731</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>732</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="C6" s="9" t="s">
         <v>733</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>734</v>
       </c>
       <c r="D6" s="9">
         <v>2007</v>
@@ -21100,16 +21647,20 @@
       <c r="G6" s="38">
         <v>0.19650000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="45">
+        <f>Table15[[#This Row],[Změna cen (%)]]/Table15[[#This Row],[Změna platů (%)]]</f>
+        <v>2.7637130801687766</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
+        <v>731</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>732</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="C7" s="9" t="s">
         <v>733</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>734</v>
       </c>
       <c r="D7" s="9">
         <v>2008</v>
@@ -21123,16 +21674,20 @@
       <c r="G7" s="38">
         <v>0.17829999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" s="46">
+        <f>Table15[[#This Row],[Změna cen (%)]]/Table15[[#This Row],[Změna platů (%)]]</f>
+        <v>1.9151450053705692</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
+        <v>731</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>732</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="C8" s="9" t="s">
         <v>733</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>734</v>
       </c>
       <c r="D8" s="9">
         <v>2009</v>
@@ -21146,16 +21701,20 @@
       <c r="G8" s="38">
         <v>0.1043</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" s="46">
+        <f>Table15[[#This Row],[Změna cen (%)]]/Table15[[#This Row],[Změna platů (%)]]</f>
+        <v>1.5428994082840239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
+        <v>731</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>732</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="C9" s="9" t="s">
         <v>733</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>734</v>
       </c>
       <c r="D9" s="9">
         <v>2015</v>
@@ -21169,16 +21728,20 @@
       <c r="G9" s="38">
         <v>0.18990000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" s="46">
+        <f>Table15[[#This Row],[Změna cen (%)]]/Table15[[#This Row],[Změna platů (%)]]</f>
+        <v>3.3141361256544508</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
+        <v>731</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>732</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>733</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>734</v>
       </c>
       <c r="D10" s="9">
         <v>2016</v>
@@ -21192,16 +21755,20 @@
       <c r="G10" s="38">
         <v>9.6199999999999994E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" s="46">
+        <f>Table15[[#This Row],[Změna cen (%)]]/Table15[[#This Row],[Změna platů (%)]]</f>
+        <v>1.6060100166944906</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
+        <v>731</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>732</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="C11" s="9" t="s">
         <v>733</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>734</v>
       </c>
       <c r="D11" s="9">
         <v>2017</v>
@@ -21215,16 +21782,20 @@
       <c r="G11" s="38">
         <v>0.1386</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" s="46">
+        <f>Table15[[#This Row],[Změna cen (%)]]/Table15[[#This Row],[Změna platů (%)]]</f>
+        <v>1.9303621169916434</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
+        <v>731</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>732</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="C12" s="19" t="s">
         <v>733</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>734</v>
       </c>
       <c r="D12" s="19">
         <v>2018</v>
@@ -21238,86 +21809,186 @@
       <c r="G12" s="40">
         <v>0.1381</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="68" t="s">
-        <v>722</v>
-      </c>
-      <c r="B50" s="69"/>
-      <c r="C50" s="69"/>
-      <c r="D50" s="69"/>
-      <c r="E50" s="69"/>
-      <c r="F50" s="69"/>
-      <c r="G50" s="70"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="71"/>
-      <c r="B51" s="72"/>
-      <c r="C51" s="72"/>
-      <c r="D51" s="72"/>
-      <c r="E51" s="72"/>
-      <c r="F51" s="72"/>
-      <c r="G51" s="73"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="71"/>
-      <c r="B52" s="72"/>
-      <c r="C52" s="72"/>
-      <c r="D52" s="72"/>
-      <c r="E52" s="72"/>
-      <c r="F52" s="72"/>
-      <c r="G52" s="73"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="74"/>
-      <c r="B53" s="75"/>
-      <c r="C53" s="75"/>
-      <c r="D53" s="75"/>
-      <c r="E53" s="75"/>
-      <c r="F53" s="75"/>
-      <c r="G53" s="76"/>
+      <c r="H12" s="47">
+        <f>Table15[[#This Row],[Změna cen (%)]]/Table15[[#This Row],[Změna platů (%)]]</f>
+        <v>1.8005215123859191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="18"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="48" t="s">
+        <v>766</v>
+      </c>
+      <c r="H13" s="49">
+        <f>AVERAGE(Table15[Poměr růstu cen a platů])</f>
+        <v>2.1246838950785536</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="88" t="s">
+        <v>768</v>
+      </c>
+      <c r="B70" s="89"/>
+      <c r="C70" s="89"/>
+      <c r="D70" s="89"/>
+      <c r="E70" s="89"/>
+      <c r="F70" s="89"/>
+      <c r="G70" s="89"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" s="87"/>
+      <c r="B71" s="87"/>
+      <c r="C71" s="87"/>
+      <c r="D71" s="87"/>
+      <c r="E71" s="87"/>
+      <c r="F71" s="87"/>
+      <c r="G71" s="87"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" s="87"/>
+      <c r="B72" s="87"/>
+      <c r="C72" s="87"/>
+      <c r="D72" s="87"/>
+      <c r="E72" s="87"/>
+      <c r="F72" s="87"/>
+      <c r="G72" s="87"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" s="87"/>
+      <c r="B73" s="87"/>
+      <c r="C73" s="87"/>
+      <c r="D73" s="87"/>
+      <c r="E73" s="87"/>
+      <c r="F73" s="87"/>
+      <c r="G73" s="87"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" s="87"/>
+      <c r="B74" s="87"/>
+      <c r="C74" s="87"/>
+      <c r="D74" s="87"/>
+      <c r="E74" s="87"/>
+      <c r="F74" s="87"/>
+      <c r="G74" s="87"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" s="87"/>
+      <c r="B75" s="87"/>
+      <c r="C75" s="87"/>
+      <c r="D75" s="87"/>
+      <c r="E75" s="87"/>
+      <c r="F75" s="87"/>
+      <c r="G75" s="87"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" s="87"/>
+      <c r="B76" s="87"/>
+      <c r="C76" s="87"/>
+      <c r="D76" s="87"/>
+      <c r="E76" s="87"/>
+      <c r="F76" s="87"/>
+      <c r="G76" s="87"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" s="87"/>
+      <c r="B77" s="87"/>
+      <c r="C77" s="87"/>
+      <c r="D77" s="87"/>
+      <c r="E77" s="87"/>
+      <c r="F77" s="87"/>
+      <c r="G77" s="87"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78" s="87"/>
+      <c r="B78" s="87"/>
+      <c r="C78" s="87"/>
+      <c r="D78" s="87"/>
+      <c r="E78" s="87"/>
+      <c r="F78" s="87"/>
+      <c r="G78" s="87"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79" s="87"/>
+      <c r="B79" s="87"/>
+      <c r="C79" s="87"/>
+      <c r="D79" s="87"/>
+      <c r="E79" s="87"/>
+      <c r="F79" s="87"/>
+      <c r="G79" s="87"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" s="87"/>
+      <c r="B80" s="87"/>
+      <c r="C80" s="87"/>
+      <c r="D80" s="87"/>
+      <c r="E80" s="87"/>
+      <c r="F80" s="87"/>
+      <c r="G80" s="87"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" s="87"/>
+      <c r="B81" s="87"/>
+      <c r="C81" s="87"/>
+      <c r="D81" s="87"/>
+      <c r="E81" s="87"/>
+      <c r="F81" s="87"/>
+      <c r="G81" s="87"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82" s="87"/>
+      <c r="B82" s="87"/>
+      <c r="C82" s="87"/>
+      <c r="D82" s="87"/>
+      <c r="E82" s="87"/>
+      <c r="F82" s="87"/>
+      <c r="G82" s="87"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A83" s="44"/>
+      <c r="B83" s="44"/>
+      <c r="C83" s="44"/>
+      <c r="D83" s="44"/>
+      <c r="E83" s="44"/>
+      <c r="F83" s="44"/>
+      <c r="G83" s="44"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84" s="44"/>
+      <c r="B84" s="44"/>
+      <c r="C84" s="44"/>
+      <c r="D84" s="44"/>
+      <c r="E84" s="44"/>
+      <c r="F84" s="44"/>
+      <c r="G84" s="44"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85" s="44"/>
+      <c r="B85" s="44"/>
+      <c r="C85" s="44"/>
+      <c r="D85" s="44"/>
+      <c r="E85" s="44"/>
+      <c r="F85" s="44"/>
+      <c r="G85" s="44"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86" s="44"/>
+      <c r="B86" s="44"/>
+      <c r="C86" s="44"/>
+      <c r="D86" s="44"/>
+      <c r="E86" s="44"/>
+      <c r="F86" s="44"/>
+      <c r="G86" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A50:G53"/>
     <mergeCell ref="A1:G3"/>
+    <mergeCell ref="A70:G82"/>
   </mergeCells>
-  <conditionalFormatting sqref="E6:E12">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F6:F12">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6:G12">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -21335,14 +22006,7 @@
   <dimension ref="A1:N235"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A59" sqref="A49:A67"/>
-      <pivotSelection pane="bottomRight" showHeader="1" axis="axisRow" activeRow="58" previousRow="58" click="1" r:id="rId3">
-        <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-          <references count="1">
-            <reference field="1" count="0"/>
-          </references>
-        </pivotArea>
-      </pivotSelection>
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -21434,22 +22098,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="55"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="61"/>
     </row>
     <row r="2" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="4"/>
@@ -24197,86 +24861,86 @@
       <c r="N69"/>
     </row>
     <row r="70" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="44" t="s">
+      <c r="A70" s="50" t="s">
         <v>489</v>
       </c>
-      <c r="B70" s="45"/>
-      <c r="C70" s="45"/>
-      <c r="D70" s="45"/>
-      <c r="E70" s="45"/>
-      <c r="F70" s="45"/>
-      <c r="G70" s="45"/>
-      <c r="H70" s="45"/>
-      <c r="I70" s="45"/>
-      <c r="J70" s="45"/>
-      <c r="K70" s="45"/>
-      <c r="L70" s="45"/>
-      <c r="M70" s="45"/>
-      <c r="N70" s="46"/>
+      <c r="B70" s="51"/>
+      <c r="C70" s="51"/>
+      <c r="D70" s="51"/>
+      <c r="E70" s="51"/>
+      <c r="F70" s="51"/>
+      <c r="G70" s="51"/>
+      <c r="H70" s="51"/>
+      <c r="I70" s="51"/>
+      <c r="J70" s="51"/>
+      <c r="K70" s="51"/>
+      <c r="L70" s="51"/>
+      <c r="M70" s="51"/>
+      <c r="N70" s="52"/>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A71" s="47"/>
-      <c r="B71" s="48"/>
-      <c r="C71" s="48"/>
-      <c r="D71" s="48"/>
-      <c r="E71" s="48"/>
-      <c r="F71" s="48"/>
-      <c r="G71" s="48"/>
-      <c r="H71" s="48"/>
-      <c r="I71" s="48"/>
-      <c r="J71" s="48"/>
-      <c r="K71" s="48"/>
-      <c r="L71" s="48"/>
-      <c r="M71" s="48"/>
-      <c r="N71" s="49"/>
+      <c r="A71" s="53"/>
+      <c r="B71" s="54"/>
+      <c r="C71" s="54"/>
+      <c r="D71" s="54"/>
+      <c r="E71" s="54"/>
+      <c r="F71" s="54"/>
+      <c r="G71" s="54"/>
+      <c r="H71" s="54"/>
+      <c r="I71" s="54"/>
+      <c r="J71" s="54"/>
+      <c r="K71" s="54"/>
+      <c r="L71" s="54"/>
+      <c r="M71" s="54"/>
+      <c r="N71" s="55"/>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A72" s="47"/>
-      <c r="B72" s="48"/>
-      <c r="C72" s="48"/>
-      <c r="D72" s="48"/>
-      <c r="E72" s="48"/>
-      <c r="F72" s="48"/>
-      <c r="G72" s="48"/>
-      <c r="H72" s="48"/>
-      <c r="I72" s="48"/>
-      <c r="J72" s="48"/>
-      <c r="K72" s="48"/>
-      <c r="L72" s="48"/>
-      <c r="M72" s="48"/>
-      <c r="N72" s="49"/>
+      <c r="A72" s="53"/>
+      <c r="B72" s="54"/>
+      <c r="C72" s="54"/>
+      <c r="D72" s="54"/>
+      <c r="E72" s="54"/>
+      <c r="F72" s="54"/>
+      <c r="G72" s="54"/>
+      <c r="H72" s="54"/>
+      <c r="I72" s="54"/>
+      <c r="J72" s="54"/>
+      <c r="K72" s="54"/>
+      <c r="L72" s="54"/>
+      <c r="M72" s="54"/>
+      <c r="N72" s="55"/>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A73" s="47"/>
-      <c r="B73" s="48"/>
-      <c r="C73" s="48"/>
-      <c r="D73" s="48"/>
-      <c r="E73" s="48"/>
-      <c r="F73" s="48"/>
-      <c r="G73" s="48"/>
-      <c r="H73" s="48"/>
-      <c r="I73" s="48"/>
-      <c r="J73" s="48"/>
-      <c r="K73" s="48"/>
-      <c r="L73" s="48"/>
-      <c r="M73" s="48"/>
-      <c r="N73" s="49"/>
+      <c r="A73" s="53"/>
+      <c r="B73" s="54"/>
+      <c r="C73" s="54"/>
+      <c r="D73" s="54"/>
+      <c r="E73" s="54"/>
+      <c r="F73" s="54"/>
+      <c r="G73" s="54"/>
+      <c r="H73" s="54"/>
+      <c r="I73" s="54"/>
+      <c r="J73" s="54"/>
+      <c r="K73" s="54"/>
+      <c r="L73" s="54"/>
+      <c r="M73" s="54"/>
+      <c r="N73" s="55"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A74" s="50"/>
-      <c r="B74" s="51"/>
-      <c r="C74" s="51"/>
-      <c r="D74" s="51"/>
-      <c r="E74" s="51"/>
-      <c r="F74" s="51"/>
-      <c r="G74" s="51"/>
-      <c r="H74" s="51"/>
-      <c r="I74" s="51"/>
-      <c r="J74" s="51"/>
-      <c r="K74" s="51"/>
-      <c r="L74" s="51"/>
-      <c r="M74" s="51"/>
-      <c r="N74" s="52"/>
+      <c r="A74" s="56"/>
+      <c r="B74" s="57"/>
+      <c r="C74" s="57"/>
+      <c r="D74" s="57"/>
+      <c r="E74" s="57"/>
+      <c r="F74" s="57"/>
+      <c r="G74" s="57"/>
+      <c r="H74" s="57"/>
+      <c r="I74" s="57"/>
+      <c r="J74" s="57"/>
+      <c r="K74" s="57"/>
+      <c r="L74" s="57"/>
+      <c r="M74" s="57"/>
+      <c r="N74" s="58"/>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C75"/>
@@ -24853,17 +25517,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="71" t="s">
         <v>506</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="67"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="73"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
@@ -24925,73 +25589,73 @@
       <c r="A8" s="5"/>
     </row>
     <row r="22" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="56" t="s">
+      <c r="A22" s="62" t="s">
         <v>510</v>
       </c>
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="57"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="58"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="63"/>
+      <c r="G22" s="63"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="64"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
     </row>
     <row r="23" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="59"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="61"/>
+      <c r="A23" s="65"/>
+      <c r="B23" s="66"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="67"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
     </row>
     <row r="24" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="59"/>
-      <c r="B24" s="60"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="60"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="60"/>
-      <c r="H24" s="60"/>
-      <c r="I24" s="61"/>
+      <c r="A24" s="65"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="67"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
     </row>
     <row r="25" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="59"/>
-      <c r="B25" s="60"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="60"/>
-      <c r="I25" s="61"/>
+      <c r="A25" s="65"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="66"/>
+      <c r="G25" s="66"/>
+      <c r="H25" s="66"/>
+      <c r="I25" s="67"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="62"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="63"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="63"/>
-      <c r="H26" s="63"/>
-      <c r="I26" s="64"/>
+      <c r="A26" s="68"/>
+      <c r="B26" s="69"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="69"/>
+      <c r="I26" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -25362,17 +26026,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="71" t="s">
         <v>593</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="67"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="73"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
@@ -25433,73 +26097,73 @@
       <c r="B7" s="5"/>
     </row>
     <row r="9" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="62" t="s">
         <v>594</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="58"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="64"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
     </row>
     <row r="10" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="59"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="61"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="67"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
     </row>
     <row r="11" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="59"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="61"/>
+      <c r="A11" s="65"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="67"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
     </row>
     <row r="12" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="59"/>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="61"/>
+      <c r="A12" s="65"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="67"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="62"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="64"/>
+      <c r="A13" s="68"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -26060,25 +26724,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="71" t="s">
         <v>721</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="67"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="73"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="D3" s="8"/>
     </row>
@@ -26239,42 +26903,42 @@
       <c r="D16" s="8"/>
     </row>
     <row r="18" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="68" t="s">
-        <v>751</v>
-      </c>
-      <c r="B18" s="69"/>
-      <c r="C18" s="69"/>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="70"/>
+      <c r="A18" s="74" t="s">
+        <v>749</v>
+      </c>
+      <c r="B18" s="75"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="76"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="71"/>
-      <c r="B19" s="72"/>
-      <c r="C19" s="72"/>
-      <c r="D19" s="72"/>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="73"/>
+      <c r="A19" s="77"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="79"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="71"/>
-      <c r="B20" s="72"/>
-      <c r="C20" s="72"/>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="73"/>
+      <c r="A20" s="77"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="79"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="74"/>
-      <c r="B21" s="75"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="75"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="76"/>
+      <c r="A21" s="80"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="81"/>
+      <c r="G21" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -26347,258 +27011,258 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>722</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>723</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>724</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>725</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>725</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>726</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>727</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>729</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>730</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>731</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>732</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>733</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>734</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>611</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>734</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>735</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>736</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>752</v>
-      </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
+        <v>751</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>737</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>753</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>731</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>732</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>733</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>734</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>622</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>735</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>752</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>736</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>754</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
+        <v>753</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>737</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>755</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>731</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>732</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>733</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>734</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>631</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>739</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>735</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>754</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>736</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>740</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>736</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>756</v>
-      </c>
-      <c r="H4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>737</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>741</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
+        <v>731</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>732</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>733</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>734</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>685</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>741</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>735</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>742</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>736</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>743</v>
-      </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
+        <v>755</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>737</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>757</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
+        <v>731</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>732</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>733</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>734</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>694</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="F6" s="5" t="s">
+        <v>735</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>756</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>736</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>758</v>
-      </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
+        <v>757</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>737</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>759</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
+        <v>731</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>732</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>733</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>734</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>703</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>735</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>736</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>760</v>
-      </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
+        <v>759</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>737</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>761</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
+        <v>731</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>732</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>733</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>734</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>712</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>735</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>760</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>736</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>762</v>
-      </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
+        <v>761</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>737</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>763</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>738</v>
       </c>
     </row>
   </sheetData>

</xml_diff>